<commit_message>
JBDC - JBDCParent- _11_JDBCSteps testing DBUtility
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fakin\Cucumber\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Create country</t>
   </si>
@@ -36,12 +36,16 @@
   </si>
   <si>
     <t>FAILED</t>
+  </si>
+  <si>
+    <t>States testing with JDBC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -421,6 +425,50 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>